<commit_message>
Add links to the sculpteo models
</commit_message>
<xml_diff>
--- a/bill_of_materials.xlsx
+++ b/bill_of_materials.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="114">
   <si>
     <t>RJ-11</t>
   </si>
@@ -347,6 +347,18 @@
   </si>
   <si>
     <t>line</t>
+  </si>
+  <si>
+    <t>Case (top)</t>
+  </si>
+  <si>
+    <t>Case(bottom)</t>
+  </si>
+  <si>
+    <t>https://www.sculpteo.com/en/print/case2-66/AvhQv5jK?uuid=f9ZfCk0V1UJiLpptjkHjRe</t>
+  </si>
+  <si>
+    <t>https://www.sculpteo.com/en/print/bottom-989/SD7MaZaD</t>
   </si>
 </sst>
 </file>
@@ -497,7 +509,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -525,6 +537,15 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -533,7 +554,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
@@ -583,6 +604,9 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -878,10 +902,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:J34"/>
+  <dimension ref="A2:J36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="H37" sqref="H37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1495,34 +1519,72 @@
       </c>
       <c r="H31" s="1"/>
     </row>
-    <row r="32" spans="1:9">
-      <c r="A32" s="17" t="s">
+    <row r="32" spans="1:9" s="44" customFormat="1">
+      <c r="A32" s="43" t="s">
         <v>101</v>
       </c>
-      <c r="B32" s="17" t="s">
+      <c r="B32" s="43" t="s">
         <v>100</v>
       </c>
-      <c r="C32" s="2" t="s">
+      <c r="C32" s="44" t="s">
         <v>70</v>
       </c>
-      <c r="F32" s="2">
+      <c r="F32" s="44">
         <v>1</v>
       </c>
-      <c r="G32" s="2">
+      <c r="G32" s="44">
         <v>0.1</v>
       </c>
-      <c r="H32" s="1"/>
-    </row>
-    <row r="33" spans="6:8">
-      <c r="H33" s="1"/>
-    </row>
-    <row r="34" spans="6:8">
-      <c r="F34" s="2" t="s">
+      <c r="H32" s="45"/>
+    </row>
+    <row r="33" spans="1:8">
+      <c r="A33" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="B33" s="17"/>
+      <c r="E33" s="2">
+        <v>10.96</v>
+      </c>
+      <c r="F33" s="15">
+        <v>1</v>
+      </c>
+      <c r="G33" s="6">
+        <f t="shared" ref="G33:G34" si="2">E33*F33</f>
+        <v>10.96</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8">
+      <c r="A34" s="17" t="s">
+        <v>111</v>
+      </c>
+      <c r="B34" s="17"/>
+      <c r="E34" s="2">
+        <v>8.8699999999999992</v>
+      </c>
+      <c r="F34" s="15">
+        <v>1</v>
+      </c>
+      <c r="G34" s="6">
+        <f t="shared" si="2"/>
+        <v>8.8699999999999992</v>
+      </c>
+      <c r="H34" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8">
+      <c r="H35" s="1"/>
+    </row>
+    <row r="36" spans="1:8">
+      <c r="F36" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="G34" s="2">
-        <f>SUM(G3:G28)</f>
-        <v>26.839999999999996</v>
+      <c r="G36" s="2">
+        <f>SUM(G3:G34)</f>
+        <v>46.97</v>
       </c>
     </row>
   </sheetData>

</xml_diff>